<commit_message>
Entefnen von unnötigen improten
</commit_message>
<xml_diff>
--- a/Test exel.xlsx
+++ b/Test exel.xlsx
@@ -683,22 +683,22 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="n">
-        <v>0.00259</v>
+        <v>0.0026</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>21.07</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>89.25</v>
+        <v>118.12</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.00258</v>
+        <v>0.00259</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>30.74</v>
       </c>
       <c r="H4" s="6" t="n">
-        <v>93.77</v>
+        <v>123.08</v>
       </c>
     </row>
     <row r="5">
@@ -709,22 +709,22 @@
       </c>
       <c r="B5" s="5" t="inlineStr"/>
       <c r="C5" s="5" t="n">
-        <v>0.0034</v>
+        <v>0.00336</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>86.3</v>
+        <v>117.01</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.00337</v>
+        <v>0.00338</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>30.84</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>94.64</v>
+        <v>123.35</v>
       </c>
     </row>
     <row r="6">
@@ -735,22 +735,22 @@
       </c>
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="n">
-        <v>0.00262</v>
+        <v>0.00263</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>21.1</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>85.39</v>
+        <v>115.15</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0.0027</v>
+        <v>0.00267</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>30.87</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v>93.90000000000001</v>
+        <v>122.05</v>
       </c>
     </row>
     <row r="7">
@@ -761,22 +761,22 @@
       </c>
       <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="n">
-        <v>0.00341</v>
+        <v>0.00339</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>84.39</v>
+        <v>115.1</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.00345</v>
+        <v>0.00342</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>30.82</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>94.3</v>
+        <v>122.42</v>
       </c>
     </row>
     <row r="8">
@@ -793,16 +793,16 @@
         <v>20.94</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>84.2</v>
+        <v>114.52</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.00238</v>
+        <v>0.00239</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>30.77</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v>93.98</v>
+        <v>121.97</v>
       </c>
     </row>
     <row r="9">
@@ -813,13 +813,13 @@
       </c>
       <c r="B9" s="5" t="inlineStr"/>
       <c r="C9" s="5" t="n">
-        <v>0.00283</v>
+        <v>0.00278</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>84.48999999999999</v>
+        <v>114.55</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>0.00277</v>
@@ -828,7 +828,7 @@
         <v>30.69</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v>93.8</v>
+        <v>121.7</v>
       </c>
     </row>
     <row r="10">
@@ -839,22 +839,22 @@
       </c>
       <c r="B10" s="5" t="inlineStr"/>
       <c r="C10" s="5" t="n">
-        <v>0.0026</v>
+        <v>0.00265</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>21.12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>85.7</v>
+        <v>115</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.00266</v>
+        <v>0.00267</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>30.82</v>
       </c>
       <c r="H10" s="6" t="n">
-        <v>93.73999999999999</v>
+        <v>121.97</v>
       </c>
     </row>
     <row r="11">
@@ -865,22 +865,22 @@
       </c>
       <c r="B11" s="11" t="inlineStr"/>
       <c r="C11" s="11" t="n">
-        <v>0.00314</v>
+        <v>0.00311</v>
       </c>
       <c r="D11" s="11" t="n">
         <v>20.99</v>
       </c>
       <c r="E11" s="11" t="n">
-        <v>87.06999999999999</v>
+        <v>115.68</v>
       </c>
       <c r="F11" s="11" t="n">
-        <v>0.00305</v>
+        <v>0.00312</v>
       </c>
       <c r="G11" s="11" t="n">
         <v>30.72</v>
       </c>
       <c r="H11" s="12" t="n">
-        <v>92.93000000000001</v>
+        <v>121.44</v>
       </c>
     </row>
     <row r="12">
@@ -1037,22 +1037,22 @@
       </c>
       <c r="B23" s="5" t="inlineStr"/>
       <c r="C23" s="5" t="n">
-        <v>0.00273</v>
+        <v>0.00268</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0.00257</v>
+        <v>0.00259</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H23" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="24">
@@ -1063,22 +1063,22 @@
       </c>
       <c r="B24" s="5" t="inlineStr"/>
       <c r="C24" s="5" t="n">
-        <v>0.00342</v>
+        <v>0.00341</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0.0034</v>
+        <v>0.00341</v>
       </c>
       <c r="G24" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H24" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="25">
@@ -1089,22 +1089,22 @@
       </c>
       <c r="B25" s="5" t="inlineStr"/>
       <c r="C25" s="5" t="n">
-        <v>0.00259</v>
+        <v>0.0026</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>0.0027</v>
+        <v>0.00267</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H25" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="26">
@@ -1115,22 +1115,22 @@
       </c>
       <c r="B26" s="5" t="inlineStr"/>
       <c r="C26" s="5" t="n">
-        <v>0.00334</v>
+        <v>0.00336</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>0.00347</v>
+        <v>0.00344</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H26" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="27">
@@ -1141,22 +1141,22 @@
       </c>
       <c r="B27" s="5" t="inlineStr"/>
       <c r="C27" s="5" t="n">
-        <v>0.00229</v>
+        <v>0.00231</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>0.00238</v>
+        <v>0.00239</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H27" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="28">
@@ -1167,13 +1167,13 @@
       </c>
       <c r="B28" s="5" t="inlineStr"/>
       <c r="C28" s="5" t="n">
-        <v>0.00278</v>
+        <v>0.00274</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F28" s="5" t="n">
         <v>0.00277</v>
@@ -1182,7 +1182,7 @@
         <v>30.79</v>
       </c>
       <c r="H28" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="29">
@@ -1193,22 +1193,22 @@
       </c>
       <c r="B29" s="5" t="inlineStr"/>
       <c r="C29" s="5" t="n">
-        <v>0.00259</v>
+        <v>0.00264</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>0.00265</v>
+        <v>0.00266</v>
       </c>
       <c r="G29" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="H29" s="6" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
     <row r="30">
@@ -1219,22 +1219,22 @@
       </c>
       <c r="B30" s="11" t="inlineStr"/>
       <c r="C30" s="11" t="n">
-        <v>0.0032</v>
+        <v>0.00312</v>
       </c>
       <c r="D30" s="11" t="n">
         <v>21</v>
       </c>
       <c r="E30" s="11" t="n">
-        <v>85.84999999999999</v>
+        <v>115.64</v>
       </c>
       <c r="F30" s="11" t="n">
-        <v>0.00302</v>
+        <v>0.00309</v>
       </c>
       <c r="G30" s="11" t="n">
         <v>30.97</v>
       </c>
       <c r="H30" s="12" t="n">
-        <v>93.88</v>
+        <v>122.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R^2 zu Data_to_excel hinzugefügt
</commit_message>
<xml_diff>
--- a/Test exel.xlsx
+++ b/Test exel.xlsx
@@ -591,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,6 +607,8 @@
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -621,7 +623,9 @@
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
       <c r="G1" s="2" t="n"/>
-      <c r="H1" s="3" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="3" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="n"/>
@@ -631,7 +635,9 @@
       <c r="E2" s="5" t="n"/>
       <c r="F2" s="5" t="n"/>
       <c r="G2" s="5" t="n"/>
-      <c r="H2" s="6" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="5" t="n"/>
+      <c r="J2" s="6" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -661,17 +667,27 @@
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
+          <t>R² Steigende Flanke</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
+        <is>
           <t>TK sinkende Flanke</t>
         </is>
       </c>
-      <c r="G3" s="8" t="inlineStr">
+      <c r="H3" s="8" t="inlineStr">
         <is>
           <t>min temp sinkende Flanke</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="I3" s="8" t="inlineStr">
         <is>
           <t>max temp sinkende Flanke</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
+        <is>
+          <t>R² sinkende Flanke</t>
         </is>
       </c>
     </row>
@@ -689,16 +705,22 @@
         <v>21.07</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>118.12</v>
+        <v>116.77</v>
       </c>
       <c r="F4" s="5" t="n">
+        <v>0.99916</v>
+      </c>
+      <c r="G4" s="5" t="n">
         <v>0.00259</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="H4" s="5" t="n">
         <v>30.74</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="I4" s="5" t="n">
         <v>123.08</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>0.99804</v>
       </c>
     </row>
     <row r="5">
@@ -715,16 +737,22 @@
         <v>20.92</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>117.01</v>
+        <v>114.17</v>
       </c>
       <c r="F5" s="5" t="n">
+        <v>0.99948</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>0.00338</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="H5" s="5" t="n">
         <v>30.84</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>123.35</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>0.99893</v>
       </c>
     </row>
     <row r="6">
@@ -735,22 +763,28 @@
       </c>
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="n">
-        <v>0.00263</v>
+        <v>0.00265</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>21.1</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>115.15</v>
+        <v>112.37</v>
       </c>
       <c r="F6" s="5" t="n">
+        <v>0.9987</v>
+      </c>
+      <c r="G6" s="5" t="n">
         <v>0.00267</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="H6" s="5" t="n">
         <v>30.87</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="I6" s="5" t="n">
         <v>122.05</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>0.99822</v>
       </c>
     </row>
     <row r="7">
@@ -767,16 +801,22 @@
         <v>20.92</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>115.1</v>
+        <v>111.71</v>
       </c>
       <c r="F7" s="5" t="n">
+        <v>0.9995000000000001</v>
+      </c>
+      <c r="G7" s="5" t="n">
         <v>0.00342</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="H7" s="5" t="n">
         <v>30.82</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="I7" s="5" t="n">
         <v>122.42</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0.99877</v>
       </c>
     </row>
     <row r="8">
@@ -793,16 +833,22 @@
         <v>20.94</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>114.52</v>
+        <v>111.32</v>
       </c>
       <c r="F8" s="5" t="n">
+        <v>0.99896</v>
+      </c>
+      <c r="G8" s="5" t="n">
         <v>0.00239</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="H8" s="5" t="n">
         <v>30.77</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="I8" s="5" t="n">
         <v>121.97</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>0.99771</v>
       </c>
     </row>
     <row r="9">
@@ -819,16 +865,22 @@
         <v>20.92</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>114.55</v>
+        <v>111.5</v>
       </c>
       <c r="F9" s="5" t="n">
+        <v>0.99951</v>
+      </c>
+      <c r="G9" s="5" t="n">
         <v>0.00277</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="H9" s="5" t="n">
         <v>30.69</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="I9" s="5" t="n">
         <v>121.7</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>0.99839</v>
       </c>
     </row>
     <row r="10">
@@ -839,22 +891,28 @@
       </c>
       <c r="B10" s="5" t="inlineStr"/>
       <c r="C10" s="5" t="n">
-        <v>0.00265</v>
+        <v>0.00264</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>21.12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>115</v>
+        <v>112.48</v>
       </c>
       <c r="F10" s="5" t="n">
+        <v>0.99881</v>
+      </c>
+      <c r="G10" s="5" t="n">
         <v>0.00267</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="H10" s="5" t="n">
         <v>30.82</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="I10" s="5" t="n">
         <v>121.97</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>0.9982</v>
       </c>
     </row>
     <row r="11">
@@ -871,16 +929,22 @@
         <v>20.99</v>
       </c>
       <c r="E11" s="11" t="n">
-        <v>115.68</v>
+        <v>113.75</v>
       </c>
       <c r="F11" s="11" t="n">
+        <v>0.99929</v>
+      </c>
+      <c r="G11" s="11" t="n">
         <v>0.00312</v>
       </c>
-      <c r="G11" s="11" t="n">
+      <c r="H11" s="11" t="n">
         <v>30.72</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="I11" s="11" t="n">
         <v>121.44</v>
+      </c>
+      <c r="J11" s="12" t="n">
+        <v>0.9982</v>
       </c>
     </row>
     <row r="12">
@@ -892,6 +956,8 @@
       <c r="F12" s="13" t="n"/>
       <c r="G12" s="13" t="n"/>
       <c r="H12" s="13" t="n"/>
+      <c r="I12" s="13" t="n"/>
+      <c r="J12" s="13" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="13" t="n"/>
@@ -902,6 +968,8 @@
       <c r="F13" s="13" t="n"/>
       <c r="G13" s="13" t="n"/>
       <c r="H13" s="13" t="n"/>
+      <c r="I13" s="13" t="n"/>
+      <c r="J13" s="13" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="13" t="n"/>
@@ -912,6 +980,8 @@
       <c r="F14" s="13" t="n"/>
       <c r="G14" s="13" t="n"/>
       <c r="H14" s="13" t="n"/>
+      <c r="I14" s="13" t="n"/>
+      <c r="J14" s="13" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="13" t="n"/>
@@ -922,6 +992,8 @@
       <c r="F15" s="13" t="n"/>
       <c r="G15" s="13" t="n"/>
       <c r="H15" s="13" t="n"/>
+      <c r="I15" s="13" t="n"/>
+      <c r="J15" s="13" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="13" t="n"/>
@@ -932,6 +1004,8 @@
       <c r="F16" s="13" t="n"/>
       <c r="G16" s="13" t="n"/>
       <c r="H16" s="13" t="n"/>
+      <c r="I16" s="13" t="n"/>
+      <c r="J16" s="13" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="13" t="n"/>
@@ -942,6 +1016,8 @@
       <c r="F17" s="13" t="n"/>
       <c r="G17" s="13" t="n"/>
       <c r="H17" s="13" t="n"/>
+      <c r="I17" s="13" t="n"/>
+      <c r="J17" s="13" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="13" t="n"/>
@@ -952,6 +1028,8 @@
       <c r="F18" s="13" t="n"/>
       <c r="G18" s="13" t="n"/>
       <c r="H18" s="13" t="n"/>
+      <c r="I18" s="13" t="n"/>
+      <c r="J18" s="13" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="13" t="n"/>
@@ -962,6 +1040,8 @@
       <c r="F19" s="13" t="n"/>
       <c r="G19" s="13" t="n"/>
       <c r="H19" s="13" t="n"/>
+      <c r="I19" s="13" t="n"/>
+      <c r="J19" s="13" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -975,7 +1055,9 @@
       <c r="E20" s="2" t="n"/>
       <c r="F20" s="2" t="n"/>
       <c r="G20" s="2" t="n"/>
-      <c r="H20" s="3" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="n"/>
+      <c r="J20" s="3" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n"/>
@@ -985,7 +1067,9 @@
       <c r="E21" s="5" t="n"/>
       <c r="F21" s="5" t="n"/>
       <c r="G21" s="5" t="n"/>
-      <c r="H21" s="6" t="n"/>
+      <c r="H21" s="5" t="n"/>
+      <c r="I21" s="5" t="n"/>
+      <c r="J21" s="6" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
@@ -1015,17 +1099,27 @@
       </c>
       <c r="F22" s="8" t="inlineStr">
         <is>
+          <t>R² Steigende Flanke</t>
+        </is>
+      </c>
+      <c r="G22" s="8" t="inlineStr">
+        <is>
           <t>TK sinkende Flanke</t>
         </is>
       </c>
-      <c r="G22" s="8" t="inlineStr">
+      <c r="H22" s="8" t="inlineStr">
         <is>
           <t>min temp sinkende Flanke</t>
         </is>
       </c>
-      <c r="H22" s="9" t="inlineStr">
+      <c r="I22" s="8" t="inlineStr">
         <is>
           <t>max temp sinkende Flanke</t>
+        </is>
+      </c>
+      <c r="J22" s="9" t="inlineStr">
+        <is>
+          <t>R² sinkende Flanke</t>
         </is>
       </c>
     </row>
@@ -1037,22 +1131,28 @@
       </c>
       <c r="B23" s="5" t="inlineStr"/>
       <c r="C23" s="5" t="n">
-        <v>0.00268</v>
+        <v>0.00271</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F23" s="5" t="n">
+        <v>0.99939</v>
+      </c>
+      <c r="G23" s="5" t="n">
         <v>0.00259</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="H23" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H23" s="6" t="n">
+      <c r="I23" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J23" s="6" t="n">
+        <v>0.99796</v>
       </c>
     </row>
     <row r="24">
@@ -1063,22 +1163,28 @@
       </c>
       <c r="B24" s="5" t="inlineStr"/>
       <c r="C24" s="5" t="n">
-        <v>0.00341</v>
+        <v>0.0034</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F24" s="5" t="n">
+        <v>0.99949</v>
+      </c>
+      <c r="G24" s="5" t="n">
         <v>0.00341</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="H24" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H24" s="6" t="n">
+      <c r="I24" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J24" s="6" t="n">
+        <v>0.99893</v>
       </c>
     </row>
     <row r="25">
@@ -1089,22 +1195,28 @@
       </c>
       <c r="B25" s="5" t="inlineStr"/>
       <c r="C25" s="5" t="n">
-        <v>0.0026</v>
+        <v>0.00262</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F25" s="5" t="n">
+        <v>0.99881</v>
+      </c>
+      <c r="G25" s="5" t="n">
         <v>0.00267</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="H25" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H25" s="6" t="n">
+      <c r="I25" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J25" s="6" t="n">
+        <v>0.9982</v>
       </c>
     </row>
     <row r="26">
@@ -1115,22 +1227,28 @@
       </c>
       <c r="B26" s="5" t="inlineStr"/>
       <c r="C26" s="5" t="n">
-        <v>0.00336</v>
+        <v>0.00335</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F26" s="5" t="n">
+        <v>0.9994499999999999</v>
+      </c>
+      <c r="G26" s="5" t="n">
         <v>0.00344</v>
       </c>
-      <c r="G26" s="5" t="n">
+      <c r="H26" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H26" s="6" t="n">
+      <c r="I26" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J26" s="6" t="n">
+        <v>0.99878</v>
       </c>
     </row>
     <row r="27">
@@ -1141,22 +1259,28 @@
       </c>
       <c r="B27" s="5" t="inlineStr"/>
       <c r="C27" s="5" t="n">
-        <v>0.00231</v>
+        <v>0.0023</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F27" s="5" t="n">
+        <v>0.99879</v>
+      </c>
+      <c r="G27" s="5" t="n">
         <v>0.00239</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="H27" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H27" s="6" t="n">
+      <c r="I27" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J27" s="6" t="n">
+        <v>0.9977200000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1173,16 +1297,22 @@
         <v>21</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F28" s="5" t="n">
+        <v>0.9996</v>
+      </c>
+      <c r="G28" s="5" t="n">
         <v>0.00277</v>
       </c>
-      <c r="G28" s="5" t="n">
+      <c r="H28" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H28" s="6" t="n">
+      <c r="I28" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J28" s="6" t="n">
+        <v>0.9984</v>
       </c>
     </row>
     <row r="29">
@@ -1193,22 +1323,28 @@
       </c>
       <c r="B29" s="5" t="inlineStr"/>
       <c r="C29" s="5" t="n">
-        <v>0.00264</v>
+        <v>0.00262</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F29" s="5" t="n">
+        <v>0.99881</v>
+      </c>
+      <c r="G29" s="5" t="n">
         <v>0.00266</v>
       </c>
-      <c r="G29" s="5" t="n">
+      <c r="H29" s="5" t="n">
         <v>30.79</v>
       </c>
-      <c r="H29" s="6" t="n">
+      <c r="I29" s="5" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J29" s="6" t="n">
+        <v>0.99821</v>
       </c>
     </row>
     <row r="30">
@@ -1219,28 +1355,34 @@
       </c>
       <c r="B30" s="11" t="inlineStr"/>
       <c r="C30" s="11" t="n">
-        <v>0.00312</v>
+        <v>0.00313</v>
       </c>
       <c r="D30" s="11" t="n">
         <v>21</v>
       </c>
       <c r="E30" s="11" t="n">
-        <v>115.64</v>
+        <v>113.01</v>
       </c>
       <c r="F30" s="11" t="n">
+        <v>0.99891</v>
+      </c>
+      <c r="G30" s="11" t="n">
         <v>0.00309</v>
       </c>
-      <c r="G30" s="11" t="n">
+      <c r="H30" s="11" t="n">
         <v>30.97</v>
       </c>
-      <c r="H30" s="12" t="n">
+      <c r="I30" s="11" t="n">
         <v>122.25</v>
+      </c>
+      <c r="J30" s="12" t="n">
+        <v>0.99817</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A20:J20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
alle werte zurück setzten wenn ne neue plotauswahl erzeugt wird
</commit_message>
<xml_diff>
--- a/Test exel.xlsx
+++ b/Test exel.xlsx
@@ -699,28 +699,28 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="n">
-        <v>0.0026</v>
+        <v>0.00256</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>21.07</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>116.77</v>
+        <v>122.42</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.99916</v>
+        <v>0.99874</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0.00259</v>
+        <v>0.00261</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>30.74</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>123.08</v>
+        <v>124.52</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>0.99804</v>
+        <v>0.99852</v>
       </c>
     </row>
     <row r="5">
@@ -731,28 +731,28 @@
       </c>
       <c r="B5" s="5" t="inlineStr"/>
       <c r="C5" s="5" t="n">
-        <v>0.00336</v>
+        <v>0.00334</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>114.17</v>
+        <v>121.76</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.99948</v>
+        <v>0.99955</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.00338</v>
+        <v>0.00339</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>30.84</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>123.35</v>
+        <v>124.04</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>0.99893</v>
+        <v>0.99922</v>
       </c>
     </row>
     <row r="6">
@@ -763,28 +763,28 @@
       </c>
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="n">
-        <v>0.00265</v>
+        <v>0.0026</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>21.1</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>112.37</v>
+        <v>120.16</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0.9987</v>
+        <v>0.99859</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0.00267</v>
+        <v>0.0027</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>30.87</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>122.05</v>
+        <v>122.69</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>0.99822</v>
+        <v>0.9987</v>
       </c>
     </row>
     <row r="7">
@@ -795,28 +795,28 @@
       </c>
       <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="n">
-        <v>0.00339</v>
+        <v>0.00341</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>111.71</v>
+        <v>120.48</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.9995000000000001</v>
+        <v>0.9996</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.00342</v>
+        <v>0.00343</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>30.82</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>122.42</v>
+        <v>122.79</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>0.99877</v>
+        <v>0.99919</v>
       </c>
     </row>
     <row r="8">
@@ -827,28 +827,28 @@
       </c>
       <c r="B8" s="5" t="inlineStr"/>
       <c r="C8" s="5" t="n">
-        <v>0.00234</v>
+        <v>0.00235</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>20.94</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>111.32</v>
+        <v>119.9</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.99896</v>
+        <v>0.99939</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.00239</v>
+        <v>0.00241</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>30.77</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>121.97</v>
+        <v>122.37</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>0.99771</v>
+        <v>0.99843</v>
       </c>
     </row>
     <row r="9">
@@ -859,28 +859,28 @@
       </c>
       <c r="B9" s="5" t="inlineStr"/>
       <c r="C9" s="5" t="n">
-        <v>0.00278</v>
+        <v>0.00276</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>20.92</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>111.5</v>
+        <v>119.79</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0.99951</v>
+        <v>0.99961</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0.00277</v>
+        <v>0.00278</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>30.69</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>121.7</v>
+        <v>122.18</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>0.99839</v>
+        <v>0.9988899999999999</v>
       </c>
     </row>
     <row r="10">
@@ -891,28 +891,28 @@
       </c>
       <c r="B10" s="5" t="inlineStr"/>
       <c r="C10" s="5" t="n">
-        <v>0.00264</v>
+        <v>0.00263</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>21.12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>112.48</v>
+        <v>120.06</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.99881</v>
+        <v>0.99866</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.00267</v>
+        <v>0.00269</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>30.82</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>121.97</v>
+        <v>122.55</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>0.9982</v>
+        <v>0.99866</v>
       </c>
     </row>
     <row r="11">
@@ -923,28 +923,28 @@
       </c>
       <c r="B11" s="11" t="inlineStr"/>
       <c r="C11" s="11" t="n">
-        <v>0.00311</v>
+        <v>0.00308</v>
       </c>
       <c r="D11" s="11" t="n">
         <v>20.99</v>
       </c>
       <c r="E11" s="11" t="n">
-        <v>113.75</v>
+        <v>120.19</v>
       </c>
       <c r="F11" s="11" t="n">
-        <v>0.99929</v>
+        <v>0.99943</v>
       </c>
       <c r="G11" s="11" t="n">
-        <v>0.00312</v>
+        <v>0.00314</v>
       </c>
       <c r="H11" s="11" t="n">
         <v>30.72</v>
       </c>
       <c r="I11" s="11" t="n">
-        <v>121.44</v>
+        <v>122.39</v>
       </c>
       <c r="J11" s="12" t="n">
-        <v>0.9982</v>
+        <v>0.99869</v>
       </c>
     </row>
     <row r="12">
@@ -1131,28 +1131,28 @@
       </c>
       <c r="B23" s="5" t="inlineStr"/>
       <c r="C23" s="5" t="n">
-        <v>0.00271</v>
+        <v>0.00259</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0.99939</v>
+        <v>0.9968900000000001</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>0.00259</v>
+        <v>0.00263</v>
       </c>
       <c r="H23" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J23" s="6" t="n">
-        <v>0.99796</v>
+        <v>0.9983300000000001</v>
       </c>
     </row>
     <row r="24">
@@ -1163,28 +1163,28 @@
       </c>
       <c r="B24" s="5" t="inlineStr"/>
       <c r="C24" s="5" t="n">
-        <v>0.0034</v>
+        <v>0.00339</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0.99949</v>
+        <v>0.99955</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>0.00341</v>
+        <v>0.00342</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J24" s="6" t="n">
-        <v>0.99893</v>
+        <v>0.99923</v>
       </c>
     </row>
     <row r="25">
@@ -1195,28 +1195,28 @@
       </c>
       <c r="B25" s="5" t="inlineStr"/>
       <c r="C25" s="5" t="n">
-        <v>0.00262</v>
+        <v>0.00258</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>0.99881</v>
+        <v>0.99877</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>0.00267</v>
+        <v>0.00269</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J25" s="6" t="n">
-        <v>0.9982</v>
+        <v>0.9987200000000001</v>
       </c>
     </row>
     <row r="26">
@@ -1227,16 +1227,16 @@
       </c>
       <c r="B26" s="5" t="inlineStr"/>
       <c r="C26" s="5" t="n">
-        <v>0.00335</v>
+        <v>0.00341</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>0.9994499999999999</v>
+        <v>0.99918</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>0.00344</v>
@@ -1245,10 +1245,10 @@
         <v>30.79</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J26" s="6" t="n">
-        <v>0.99878</v>
+        <v>0.9992</v>
       </c>
     </row>
     <row r="27">
@@ -1259,28 +1259,28 @@
       </c>
       <c r="B27" s="5" t="inlineStr"/>
       <c r="C27" s="5" t="n">
-        <v>0.0023</v>
+        <v>0.00234</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>0.99879</v>
+        <v>0.99898</v>
       </c>
       <c r="G27" s="5" t="n">
-        <v>0.00239</v>
+        <v>0.00241</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J27" s="6" t="n">
-        <v>0.9977200000000001</v>
+        <v>0.99843</v>
       </c>
     </row>
     <row r="28">
@@ -1297,10 +1297,10 @@
         <v>21</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>0.9996</v>
+        <v>0.9996699999999999</v>
       </c>
       <c r="G28" s="5" t="n">
         <v>0.00277</v>
@@ -1309,10 +1309,10 @@
         <v>30.79</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J28" s="6" t="n">
-        <v>0.9984</v>
+        <v>0.9989</v>
       </c>
     </row>
     <row r="29">
@@ -1323,28 +1323,28 @@
       </c>
       <c r="B29" s="5" t="inlineStr"/>
       <c r="C29" s="5" t="n">
-        <v>0.00262</v>
+        <v>0.00261</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>0.99881</v>
+        <v>0.9987</v>
       </c>
       <c r="G29" s="5" t="n">
-        <v>0.00266</v>
+        <v>0.00268</v>
       </c>
       <c r="H29" s="5" t="n">
         <v>30.79</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J29" s="6" t="n">
-        <v>0.99821</v>
+        <v>0.99866</v>
       </c>
     </row>
     <row r="30">
@@ -1355,28 +1355,28 @@
       </c>
       <c r="B30" s="11" t="inlineStr"/>
       <c r="C30" s="11" t="n">
-        <v>0.00313</v>
+        <v>0.00306</v>
       </c>
       <c r="D30" s="11" t="n">
         <v>21</v>
       </c>
       <c r="E30" s="11" t="n">
-        <v>113.01</v>
+        <v>120.49</v>
       </c>
       <c r="F30" s="11" t="n">
-        <v>0.99891</v>
+        <v>0.9986</v>
       </c>
       <c r="G30" s="11" t="n">
-        <v>0.00309</v>
+        <v>0.00312</v>
       </c>
       <c r="H30" s="11" t="n">
         <v>30.97</v>
       </c>
       <c r="I30" s="11" t="n">
-        <v>122.25</v>
+        <v>122.9</v>
       </c>
       <c r="J30" s="12" t="n">
-        <v>0.99817</v>
+        <v>0.99857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>